<commit_message>
setLevel Functions in FunctionMap
</commit_message>
<xml_diff>
--- a/FunctionMap.xlsx
+++ b/FunctionMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fisherd\Desktop\Projects\CREDA\CREDA_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86F04262-AD96-4C3B-805C-210A9477496C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628DA1FF-FC6B-431C-BFFE-A18DB75A15DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="171">
   <si>
     <t>TempID</t>
   </si>
@@ -604,6 +604,18 @@
   </si>
   <si>
     <t>Michigan address (unimplemented)</t>
+  </si>
+  <si>
+    <t>helper.setVerbose()</t>
+  </si>
+  <si>
+    <t>helper.setSilent()</t>
+  </si>
+  <si>
+    <t>No. This function changes settings so functions run silently</t>
+  </si>
+  <si>
+    <t>No. This function changes settings so functions run in verbose mode</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1016,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11"/>
+      <selection pane="topRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2057,12 @@
       <c r="AD25" s="1"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
+      <c r="A26" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
@@ -2063,7 +2080,12 @@
       <c r="AD26" s="1"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
+      <c r="A27" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>

</xml_diff>

<commit_message>
polishing. Removed flushing error
</commit_message>
<xml_diff>
--- a/FunctionMap.xlsx
+++ b/FunctionMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fisherd\Desktop\Projects\CREDA\CREDA_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628DA1FF-FC6B-431C-BFFE-A18DB75A15DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19551432-5B6D-425F-8448-1A95E558763E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed View" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="169">
   <si>
     <t>TempID</t>
   </si>
@@ -480,12 +480,6 @@
     <t>Yes. Accepts a shapefile as input, and creates a serialized Python object for rapid shape loading later</t>
   </si>
   <si>
-    <t>helper.CREDA_Project("UBIDs", infile)</t>
-  </si>
-  <si>
-    <t>No. UBID record in memory in memory. All provided shapes are best_matches by default</t>
-  </si>
-  <si>
     <t>AddrInf_01</t>
   </si>
   <si>
@@ -558,9 +552,6 @@
     <t>Invalid shape format</t>
   </si>
   <si>
-    <t>Shape combining multiple lines</t>
-  </si>
-  <si>
     <t>Bad WKT string</t>
   </si>
   <si>
@@ -597,9 +588,6 @@
     <t>Doesn't cause program to stop. Just flags the bad record</t>
   </si>
   <si>
-    <t>Set whenever multiple lines are connected by a single ShapeID (useful for Shapefile without preprocessing)</t>
-  </si>
-  <si>
     <t>AddrInf_06</t>
   </si>
   <si>
@@ -616,6 +604,12 @@
   </si>
   <si>
     <t>No. This function changes settings so functions run in verbose mode</t>
+  </si>
+  <si>
+    <t>Multipolygon record</t>
+  </si>
+  <si>
+    <t>Set whenever multiple ShapeIDZs are connected by a single ShapeID via multipolgon input</t>
   </si>
 </sst>
 </file>
@@ -1014,41 +1008,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AD47"/>
+  <dimension ref="A3:AD46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B27" sqref="B27"/>
+      <selection pane="topRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="23" width="8.140625" customWidth="1"/>
-    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="23" width="8.109375" customWidth="1"/>
+    <col min="24" max="24" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C3" s="15" t="s">
         <v>57</v>
       </c>
@@ -1094,9 +1088,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -1135,10 +1129,10 @@
         <v>61</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>63</v>
@@ -1180,7 +1174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>43</v>
       </c>
@@ -1223,7 +1217,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1270,7 +1264,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1313,7 +1307,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1354,7 +1348,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1404,7 +1398,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1442,7 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -1494,7 +1488,7 @@
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1538,7 +1532,7 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1591,7 +1585,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1653,7 +1647,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1697,7 +1691,7 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
@@ -1755,7 +1749,7 @@
       <c r="AC16" s="7"/>
       <c r="AD16" s="7"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>26</v>
       </c>
@@ -1794,68 +1788,59 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>125</v>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="N18" s="1"/>
       <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
-      <c r="Z18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB18" s="14"/>
-      <c r="AC18" s="14"/>
-      <c r="AD18" s="14"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="P18" s="1"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="N19" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="N19" s="7"/>
       <c r="O19" s="14"/>
-      <c r="P19" s="1"/>
+      <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
@@ -1863,34 +1848,27 @@
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="N20" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="N20" s="1"/>
       <c r="O20" s="14"/>
-      <c r="P20" s="7"/>
+      <c r="P20" s="1"/>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
@@ -1898,15 +1876,18 @@
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="7"/>
-      <c r="AB20" s="7"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1934,11 +1915,13 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B22" s="2"/>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1965,12 +1948,12 @@
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1998,21 +1981,13 @@
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+        <v>124</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="14"/>
       <c r="P24" s="1"/>
@@ -2031,15 +2006,13 @@
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="N25" s="1"/>
-      <c r="O25" s="14"/>
+        <v>166</v>
+      </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
@@ -2056,12 +2029,12 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="7"/>
@@ -2079,88 +2052,65 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>168</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2185,13 +2135,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -2199,7 +2149,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>43</v>
       </c>
@@ -2207,7 +2157,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2215,7 +2165,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -2223,7 +2173,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>44</v>
       </c>
@@ -2231,7 +2181,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -2239,7 +2189,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>76</v>
       </c>
@@ -2247,7 +2197,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>78</v>
       </c>
@@ -2255,7 +2205,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
@@ -2263,7 +2213,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
@@ -2271,7 +2221,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>15</v>
       </c>
@@ -2279,7 +2229,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>49</v>
       </c>
@@ -2287,7 +2237,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>50</v>
       </c>
@@ -2295,7 +2245,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>5</v>
       </c>
@@ -2303,7 +2253,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>0</v>
       </c>
@@ -2311,7 +2261,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>7</v>
       </c>
@@ -2319,7 +2269,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>79</v>
       </c>
@@ -2341,14 +2291,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>107</v>
       </c>
@@ -2359,7 +2309,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -2370,7 +2320,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -2381,7 +2331,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -2392,7 +2342,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2403,7 +2353,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2414,7 +2364,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -2438,13 +2388,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2452,100 +2402,100 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2562,14 +2512,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="72.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2577,48 +2527,48 @@
         <v>99</v>
       </c>
       <c r="C1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>144</v>
       </c>
-      <c r="B2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>140</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2630,18 +2580,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91181B90-A06B-4770-8D13-EA232071D336}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2649,51 +2599,51 @@
         <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>147</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>150</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>153</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FunctionMap descriptions, C and R explained
</commit_message>
<xml_diff>
--- a/FunctionMap.xlsx
+++ b/FunctionMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fisherd\Desktop\Projects\CREDA\CREDA_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19551432-5B6D-425F-8448-1A95E558763E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA76A64D-CFB6-49FB-A4A0-5C295F7C01E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed View" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author>Fisher, David</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="174">
   <si>
     <t>TempID</t>
   </si>
@@ -610,6 +610,66 @@
   </si>
   <si>
     <t>Set whenever multiple ShapeIDZs are connected by a single ShapeID via multipolgon input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sheet provides the detailed view of how we traverse the program. </t>
+  </si>
+  <si>
+    <t>Highlighted cells represent entry points (addresses, geocodes, shapes). E.g users can create a project, starting with addresses, with
+project = helper.CREDA_projects("addresses", &lt;infile&gt;)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Columns C - AB describe inputs/outputs of each step. 'R' values imply </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to run the steps, while 'C' values imply </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>created</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> by the step</t>
+    </r>
+  </si>
+  <si>
+    <t>C (Created)</t>
+  </si>
+  <si>
+    <t>R (Required)</t>
   </si>
 </sst>
 </file>
@@ -1008,21 +1068,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AD46"/>
+  <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="A18" sqref="A18:XFD18"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="60.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="104.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
     <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
@@ -1042,210 +1102,178 @@
     <col min="28" max="28" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="C3" s="15" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15" t="s">
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15" t="s">
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15" t="s">
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="O4" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="AA4" s="15"/>
       <c r="AB4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="C6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="14"/>
       <c r="P6" s="1"/>
@@ -1266,15 +1294,17 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>3</v>
+        <v>173</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>3</v>
@@ -1286,9 +1316,11 @@
         <v>3</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="14"/>
       <c r="P7" s="1"/>
@@ -1309,14 +1341,16 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1326,10 +1360,10 @@
       <c r="H8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="I8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="14"/>
       <c r="P8" s="1"/>
@@ -1350,10 +1384,10 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1370,15 +1404,6 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="14"/>
@@ -1399,20 +1424,26 @@
       <c r="AD9" s="1"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1443,36 +1474,34 @@
       <c r="AD10" s="1"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>41</v>
+      <c r="A11" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="1"/>
       <c r="O11" s="14"/>
-      <c r="P11" s="7"/>
+      <c r="P11" s="1"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
@@ -1480,43 +1509,45 @@
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>22</v>
+      <c r="A12" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N12" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="7"/>
       <c r="O12" s="14"/>
-      <c r="P12" s="1"/>
+      <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
@@ -1524,20 +1555,20 @@
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1546,37 +1577,28 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="N13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="U13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="V13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="J13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
@@ -1587,10 +1609,10 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1600,47 +1622,38 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N14" s="1"/>
+      <c r="N14" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="O14" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="W14" s="7"/>
-      <c r="X14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
@@ -1649,10 +1662,10 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1662,138 +1675,161 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="M15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="N15" s="1"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
+      <c r="O15" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="W15" s="7"/>
       <c r="X15" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O16" s="14"/>
-      <c r="P16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="R16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="U16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="V16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="7"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="C17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" s="14"/>
+      <c r="P17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1812,35 +1848,39 @@
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
+      <c r="W18" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
+      <c r="AA18" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="AB18" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="N19" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="N19" s="1"/>
       <c r="O19" s="14"/>
-      <c r="P19" s="7"/>
+      <c r="P19" s="1"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
@@ -1848,27 +1888,34 @@
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
-      <c r="AC19" s="7"/>
-      <c r="AD19" s="7"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="N20" s="7"/>
       <c r="O20" s="14"/>
-      <c r="P20" s="1"/>
+      <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
@@ -1876,18 +1923,15 @@
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1916,12 +1960,10 @@
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>120</v>
-      </c>
+      <c r="A22" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1950,10 +1992,10 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1983,11 +2025,19 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>124</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="14"/>
       <c r="P24" s="1"/>
@@ -2008,11 +2058,13 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>166</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N25" s="1"/>
+      <c r="O25" s="14"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
@@ -2031,10 +2083,10 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="7"/>
@@ -2053,7 +2105,27 @@
       <c r="AD26" s="1"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="A27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
@@ -2112,14 +2184,17 @@
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
     </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="N3:W3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="N4:W4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="X4:Y4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2580,7 +2655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91181B90-A06B-4770-8D13-EA232071D336}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>